<commit_message>
Added sprint 3 backlog
</commit_message>
<xml_diff>
--- a/SCRUM files/Agile-User-Story.xlsx
+++ b/SCRUM files/Agile-User-Story.xlsx
@@ -1131,7 +1131,9 @@
       <c r="G6" s="8">
         <v>3.0</v>
       </c>
-      <c r="H6" s="10"/>
+      <c r="H6" s="13">
+        <v>3.0</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="12" t="s">
         <v>24</v>
@@ -1173,7 +1175,9 @@
       <c r="G7" s="8">
         <v>5.0</v>
       </c>
-      <c r="H7" s="10"/>
+      <c r="H7" s="13">
+        <v>3.0</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1893,7 +1897,9 @@
       <c r="G25" s="9">
         <v>5.0</v>
       </c>
-      <c r="H25" s="10"/>
+      <c r="H25" s="13">
+        <v>3.0</v>
+      </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -2345,7 +2351,9 @@
       <c r="G36" s="8">
         <v>5.0</v>
       </c>
-      <c r="H36" s="10"/>
+      <c r="H36" s="13">
+        <v>3.0</v>
+      </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -2385,7 +2393,9 @@
       <c r="G37" s="8">
         <v>5.0</v>
       </c>
-      <c r="H37" s="10"/>
+      <c r="H37" s="13">
+        <v>3.0</v>
+      </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>

</xml_diff>